<commit_message>
feature/ADMINDASH-253: changed because API change
</commit_message>
<xml_diff>
--- a/client/assets/template/importUserOrderAttempt.xlsx
+++ b/client/assets/template/importUserOrderAttempt.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\etobee-admin\client\assets\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymondlukanta/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>EDSNumber</t>
   </si>
   <si>
-    <t>Reason</t>
-  </si>
-  <si>
-    <t>AttemptDate</t>
-  </si>
-  <si>
     <t>CONSIGNEE_DOES_NOT_HAVE_ENOUGH_CASH</t>
   </si>
   <si>
@@ -70,6 +64,18 @@
   </si>
   <si>
     <t>BAD_ADDRESS</t>
+  </si>
+  <si>
+    <t>SecondAttemptDate</t>
+  </si>
+  <si>
+    <t>SecondAttemptReason</t>
+  </si>
+  <si>
+    <t>FirstAttemptDate</t>
+  </si>
+  <si>
+    <t>FirstAttemptReason</t>
   </si>
 </sst>
 </file>
@@ -126,9 +132,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -397,43 +400,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.69921875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Perhatikan Format Penulisan" prompt="Ketik: DD/MM/YYYY_x000a_Contoh: 16/12/2016" sqref="C1:C1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Perhatikan Format Penulisan" prompt="Ketik: DD/MM/YYYY_x000a_Contoh: 16/12/2016" sqref="E1:E1048576"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet2!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B1:B1048576</xm:sqref>
+          <xm:sqref>B2:B1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet2!$A$1:$A$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -446,69 +464,69 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hotfix change template attempt
</commit_message>
<xml_diff>
--- a/client/assets/template/importUserOrderAttempt.xlsx
+++ b/client/assets/template/importUserOrderAttempt.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
-  <workbookPr showInkAnnotation="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymondlukanta/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -180,7 +175,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -215,7 +210,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -392,7 +387,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -402,11 +397,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
@@ -415,7 +408,7 @@
     <col min="5" max="5" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,14 +426,14 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Perhatikan Format Penulisan" prompt="Ketik: DD/MM/YYYY_x000a_Contoh: 16/12/2016" sqref="C1:C1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Perhatikan Format Penulisan" prompt="Ketik: DD/MM/YYYY_x000a_Contoh: 16/12/2016" sqref="E1:E1048576"/>
+  <dataValidations xWindow="242" yWindow="204" count="2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Perhatikan Format Penulisan" prompt="Ketik: MM/DD/YYYY_x000a_Contoh: 12/16/2016" sqref="C1:C1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Perhatikan Format Penulisan" prompt="Ketik: MM/DD/YYYY_x000a_Contoh: 12/16/2016" sqref="E1:E1048576"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="242" yWindow="204" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet2!$A:$A</xm:f>
@@ -455,6 +448,9 @@
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
   </extLst>
 </worksheet>
 </file>
@@ -467,69 +463,74 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update attempt import template
</commit_message>
<xml_diff>
--- a/client/assets/template/importUserOrderAttempt.xlsx
+++ b/client/assets/template/importUserOrderAttempt.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\etobee-admin\client\assets\template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="16056" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>EDSNumber</t>
   </si>
@@ -71,12 +76,66 @@
   </si>
   <si>
     <t>FirstAttemptReason</t>
+  </si>
+  <si>
+    <t>FirstAttemptProofURL</t>
+  </si>
+  <si>
+    <t>SecondAttemptProofURL</t>
+  </si>
+  <si>
+    <t>CONSIGNEE_WANT_RESCHEDULE</t>
+  </si>
+  <si>
+    <t>NATURAL_DISASTER</t>
+  </si>
+  <si>
+    <t>EKYC_FAILED</t>
+  </si>
+  <si>
+    <t>CONSIGNEE_MOVE_OUT</t>
+  </si>
+  <si>
+    <t>CONSIGNEE_NOT_RECOGNIZED</t>
+  </si>
+  <si>
+    <t>CONSIGNEE_RARELY_IN_PLACE</t>
+  </si>
+  <si>
+    <t>OFFICE_CLOSED</t>
+  </si>
+  <si>
+    <t>LEAVE_HOLIDAY_SICK</t>
+  </si>
+  <si>
+    <t>OUT_OF_TOWN</t>
+  </si>
+  <si>
+    <t>CONSIGNEE_PASSED_AWAY</t>
+  </si>
+  <si>
+    <t>CONSIGNEE_RETIRED_RESIGNED</t>
+  </si>
+  <si>
+    <t>CONSIGNEE_DIFFICULT_TO_MEET</t>
+  </si>
+  <si>
+    <t>NEGATIVE_LOCATION</t>
+  </si>
+  <si>
+    <t>INCOMPLETE_ADDRESS</t>
+  </si>
+  <si>
+    <t>PACKAGE_NOT_READY</t>
+  </si>
+  <si>
+    <t>PACKAGE_OVERSIZED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
@@ -127,6 +186,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -387,7 +449,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -395,20 +457,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.296875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="19.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.69921875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -418,17 +483,22 @@
       <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations xWindow="242" yWindow="204" count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Perhatikan Format Penulisan" prompt="Ketik: MM/DD/YYYY_x000a_Contoh: 12/16/2016" sqref="C1:C1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Perhatikan Format Penulisan" prompt="Ketik: MM/DD/YYYY_x000a_Contoh: 12/16/2016" sqref="E1:E1048576"/>
+  <dataValidations xWindow="242" yWindow="204" count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Perhatikan Format Penulisan" prompt="Ketik: MM/DD/YYYY_x000a_Contoh: 12/16/2016" sqref="C1:D1048576 F1:F1048576"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -444,7 +514,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -457,72 +527,152 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hotfix/ADMINDASH-532: error on import last mile attempt
</commit_message>
<xml_diff>
--- a/client/assets/template/importUserOrderAttempt.xlsx
+++ b/client/assets/template/importUserOrderAttempt.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\etobee-admin\client\assets\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Petrus\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="16056" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>EDSNumber</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>PACKAGE_OVERSIZED</t>
+  </si>
+  <si>
+    <t>09/09/2017 01:00:00 PM</t>
+  </si>
+  <si>
+    <t>EDSXXXXXXXX</t>
   </si>
 </sst>
 </file>
@@ -139,7 +145,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -147,16 +153,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -164,19 +196,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,23 +510,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.296875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="19.69921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.69921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.25" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.25" style="7" customWidth="1"/>
+    <col min="5" max="5" width="19.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.25" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,25 +550,45 @@
         <v>18</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations xWindow="242" yWindow="204" count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Perhatikan Format Penulisan" prompt="Ketik: MM/DD/YYYY_x000a_Contoh: 12/16/2016" sqref="C1:D1048576 F1:F1048576"/>
+  <dataValidations xWindow="286" yWindow="282" count="3">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Perhatikan Format Penulisan" prompt="Ketik: MM/DD/YYYY_x000a_Contoh: 12/16/2016" sqref="D1:D1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Perhatikan Format Penulisan" prompt="Ketik: MM/DD/YYYY hh:mm:ss a_x000a_Contoh: 06/17/2017 03:00:00 PM" sqref="C1:C1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Perhatikan Format Penulisan" prompt="Ketik: MM/DD/YYYY hh:mm:ss a_x000a_Contoh: 06/17/2017 03:00:00 PM" sqref="F1:F1048576"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="242" yWindow="204" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="286" yWindow="282" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet2!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B1048576</xm:sqref>
+          <xm:sqref>E2 B2:B1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
+          <xm:sqref>E3:E1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -529,148 +603,148 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
feature/ADMINDASH-552: Add new reason in import attempt
</commit_message>
<xml_diff>
--- a/client/assets/template/importUserOrderAttempt.xlsx
+++ b/client/assets/template/importUserOrderAttempt.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Petrus\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fadhil/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10000" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>EDSNumber</t>
   </si>
@@ -51,9 +54,6 @@
     <t>STUFF_OR_BOX_IS_BROKEN</t>
   </si>
   <si>
-    <t>DRIVER_ARRIVED_TOO_LATE</t>
-  </si>
-  <si>
     <t>COD_MISMATCH</t>
   </si>
   <si>
@@ -136,12 +136,18 @@
   </si>
   <si>
     <t>EDSXXXXXXXX</t>
+  </si>
+  <si>
+    <t>CONSIGNEE_UNKNOWN</t>
+  </si>
+  <si>
+    <t>NO_CONSIGNEE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
@@ -512,19 +518,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.25" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.25" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.25" style="7" customWidth="1"/>
-    <col min="5" max="5" width="19.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.25" style="3"/>
+    <col min="1" max="1" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.1640625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -532,39 +538,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -577,23 +583,26 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="286" yWindow="282" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="286" yWindow="282" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet2!$A$1:$A$19</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E1048576</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet2!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>E2 B2:B1048576</xm:sqref>
+          <xm:sqref>E2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Sheet2!$A$1:$A$12</xm:f>
+            <xm:f>Sheet2!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E1048576</xm:sqref>
+          <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
@@ -601,17 +610,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A28"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -631,130 +640,130 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>34</v>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>